<commit_message>
Fixed root and adjusted label for pre-eclampsia
</commit_message>
<xml_diff>
--- a/metaData/kenya-2012_vignettes_codebook.xlsx
+++ b/metaData/kenya-2012_vignettes_codebook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annak\Box Sync\WB Work\WB Github Repo\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annak\Documents\GitHub\SDI-Health\metaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{42F3FB42-8D44-4354-98B0-3F31FE1B54A7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{56ADC60E-AA2B-44BB-8291-4476C3978BB8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-21143" windowWidth="7485" windowHeight="21143" tabRatio="579" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3729,9 +3729,6 @@
     <t>Did not do pregnancy vignette</t>
   </si>
   <si>
-    <t>Did not do eclampsia vignette</t>
-  </si>
-  <si>
     <t>q131</t>
   </si>
   <si>
@@ -3793,6 +3790,9 @@
   </si>
   <si>
     <t>Did not do malaria+anemia vignette</t>
+  </si>
+  <si>
+    <t>Did not do pre-eclampsia vignette</t>
   </si>
 </sst>
 </file>
@@ -4357,8 +4357,8 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="48" zoomScaleNormal="48" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="17.25" x14ac:dyDescent="0.45"/>
@@ -4416,7 +4416,7 @@
         <v>1205</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="D4" s="10"/>
     </row>
@@ -4432,7 +4432,7 @@
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="24" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>1207</v>
@@ -4462,7 +4462,7 @@
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="24" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="B9" s="31" t="s">
         <v>1210</v>
@@ -4512,10 +4512,10 @@
     </row>
     <row r="14" spans="1:4" ht="34.5" x14ac:dyDescent="0.45">
       <c r="A14" s="23" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>1241</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>1242</v>
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="10"/>
@@ -4535,7 +4535,7 @@
         <v>1215</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="C16" s="23" t="s">
         <v>851</v>
@@ -4563,7 +4563,7 @@
         <v>1217</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="C18" s="23" t="s">
         <v>852</v>
@@ -4577,7 +4577,7 @@
         <v>1218</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="C19" s="23" t="s">
         <v>853</v>
@@ -4591,7 +4591,7 @@
         <v>1219</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>855</v>
@@ -4605,7 +4605,7 @@
         <v>1220</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>856</v>
@@ -4619,7 +4619,7 @@
         <v>1221</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="C22" s="23" t="s">
         <v>857</v>
@@ -4652,7 +4652,7 @@
         <v>1225</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>1227</v>
+        <v>1248</v>
       </c>
       <c r="D25" s="10"/>
     </row>
@@ -4669,18 +4669,18 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="23" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>1237</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>1238</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="23" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>1239</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>1240</v>
       </c>
     </row>
   </sheetData>
@@ -8014,10 +8014,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="21" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B72" s="13" t="s">
         <v>1235</v>
-      </c>
-      <c r="B72" s="13" t="s">
-        <v>1236</v>
       </c>
     </row>
   </sheetData>
@@ -15266,7 +15266,7 @@
         <v>869</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="C6" s="26" t="s">
         <v>870</v>
@@ -15274,24 +15274,24 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="26" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B7" s="26">
         <v>0</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="26" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B8" s="26">
         <v>1</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>